<commit_message>
Update : C14 Data
- 몽촌토성
</commit_message>
<xml_diff>
--- a/Data/AMS_Master.xlsx
+++ b/Data/AMS_Master.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\풍납토성발굴조사단\Desktop\주찬혁\개인\github\Pungnaptoseong_AMS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\Pungnaptoseong_AMS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2258E8A9-7945-4D2A-B528-9BE018B53885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14595" yWindow="0" windowWidth="14205" windowHeight="18000"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="21705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PNTS C14" sheetId="1" r:id="rId1"/>
@@ -23,23 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="611">
   <si>
     <t>LabID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1419,10 +1409,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>EPSG:4326, WGS84</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>시료 출토 맥락에 관한 서술</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1463,10 +1449,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>미보정된 값임</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>오차범위</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1516,14 +1498,964 @@
   </si>
   <si>
     <t>Radpion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>천호동 328-9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시료 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CWd231159</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수도문물연구원,, 2024, 천호동 328-9번지 유적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼국시대 수혈-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼국시대 구상유구-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구상유구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닥(흙 포함)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150397</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150398</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한성백제박물관, 2016, 몽촌토성Ⅰ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19호 주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20호 주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>26호 주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>27호 주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>28호 주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주혈군 B군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2지구 주혈군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2지구 우물</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2지구 1호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생활면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아궁이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재층(내부토)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닥 재층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우물 바닥면 재층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우물</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-18-04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150686</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150687</t>
+  </si>
+  <si>
+    <t>KGM-OWd150688</t>
+  </si>
+  <si>
+    <t>KGM-OWd150689</t>
+  </si>
+  <si>
+    <t>KGM-OWd150690</t>
+  </si>
+  <si>
+    <t>KGM-OWd150691</t>
+  </si>
+  <si>
+    <t>KGM-OWd150692</t>
+  </si>
+  <si>
+    <t>KGM-OWd160101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd160110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd160111</t>
+  </si>
+  <si>
+    <t>KGM-OWd160112</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-190055</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한성백제박물관, 2019, 몽촌토성Ⅲ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*EPSG:4326, WGS84</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*미보정된 값임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌15-15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-17-03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-17-15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-18-10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-17-24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-18-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-18-08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-16-22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-18-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-18-07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-17-11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-2호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-6호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-5호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-7호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-14호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-15호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-16호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-25호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-26호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-27호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-30호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-32호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-33호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-9호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-11호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-12호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-31호 수혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백제 2호 주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재층(초본류)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>황갈색 점토 상면 부뚜막 좌측</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닥면 회색점토 내 부뚜막 우측</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재층 상단(바로 위층)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추정 고래 아궁이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소결면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소결면 집석부 내부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd160103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd160104</t>
+  </si>
+  <si>
+    <t>KGM-OWd170052</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170053</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd160105</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170054</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170055</t>
+  </si>
+  <si>
+    <t>KGM-OWd170056</t>
+  </si>
+  <si>
+    <t>KGM-OWd170058</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-180172</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170059</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170060</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170067</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-180179</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170061</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170062</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170063</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-190060</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-180184</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170064</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170065</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170066</t>
+  </si>
+  <si>
+    <t>RPC-180185</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-190058</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170057</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd160106</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd160107</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd160108</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-180186</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-190057</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-180177</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한성백제박물관, 2021, 몽촌토성Ⅳ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌토성 북문지 내측(2013-2014)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌토성 북문지 일원(통일신라시대)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150402</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1pit 바닥 채취</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수혈 바닥 채취</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150403</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌토성 북서벽 구 목책 설치구간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성벽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일신라 4호 주거지-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일신라 4호 주거지-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일신라 1호 주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일신라 5호 주거지-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일신라 8호 주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일신라 10호 주거지-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일신라 11호 주거지-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일신라 13호 주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일신라 14호 주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일신라 16호 주거지-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일신라 17호 주거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기둥 내(흙 포함)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구들 바닥(17.02m)(흙 포함)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 기둥구멍 내(흙 포함)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구들 바닥(흙 포함)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구들(흙, 호일 포함)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>둑 제거중(흙 포함)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-14-14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SNU 14-046</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SNU 14-147</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150388</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KMG-OWd150389</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150390</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150391</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150392</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150393</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150394</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150395</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd150399</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌토성 북문지 일원(삼국시대 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌토성 북문지 일원(삼국시대 2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백제 생활면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-1호 벽주 건물지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>벽구 북서쪽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-5∼6호수혈 남서측 백제 생활면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고구려 문화층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-2호 벽주 건물지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8번 주혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성토대지 성토층(NW19NE13)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성토대지 성토층(NW18NE13) 그리드남측 둑 제거 중 상부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건물지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-15-14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-17-21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-17-23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-18-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌-18-5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd160102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-180181</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-180183</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-190054</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-190056</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한성백제박물관, 2023, 몽촌토성Ⅴ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성내순환도로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1호 동서도로 측구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백제 개축도로 1호 동서도로 노면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽촌토성 북문지 일원(삼국시대 3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성내순환도로 하부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1호 동서도로 측구 내 목탄층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NW16NE12 Pit 14 백제 개축도로 1호 동서도로 노면 상면 재층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>120170365-011-00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>120170365-013-00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>120170365-014-00</t>
+  </si>
+  <si>
+    <t>120170365-015-00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPC-180182</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170047</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170050</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KGM-OWd170051</t>
+  </si>
+  <si>
+    <t>한성백제박물관, 2024, 몽촌토성Ⅵ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1566,6 +2498,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -1679,7 +2619,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1713,13 +2653,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1736,6 +2676,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2070,18 +3016,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="87" workbookViewId="0">
-      <selection activeCell="I107" sqref="I107"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D204" sqref="D204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.6640625" style="7" customWidth="1"/>
     <col min="2" max="3" width="12.77734375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" style="8" customWidth="1"/>
     <col min="5" max="5" width="19.109375" style="8" customWidth="1"/>
     <col min="6" max="6" width="22.44140625" style="9" customWidth="1"/>
     <col min="7" max="7" width="11.77734375" style="7" customWidth="1"/>
@@ -6589,7 +7535,7 @@
         <v>30</v>
       </c>
       <c r="N120" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="121" spans="1:14">
@@ -6625,7 +7571,7 @@
         <v>30</v>
       </c>
       <c r="N121" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="122" spans="1:14">
@@ -6638,20 +7584,20 @@
         <v>329</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F122" s="6"/>
       <c r="G122" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I122" s="5" t="s">
         <v>117</v>
       </c>
       <c r="J122" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K122" s="4"/>
       <c r="L122" s="4">
@@ -6661,7 +7607,7 @@
         <v>30</v>
       </c>
       <c r="N122" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="123" spans="1:14">
@@ -6671,24 +7617,24 @@
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F123" s="6"/>
       <c r="G123" s="4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H123" s="5"/>
       <c r="I123" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J123" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="K123" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L123" s="4">
         <v>1700</v>
@@ -6697,7 +7643,7 @@
         <v>40</v>
       </c>
       <c r="N123" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="124" spans="1:14">
@@ -6706,20 +7652,2762 @@
       </c>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="5"/>
-      <c r="F124" s="6"/>
-      <c r="G124" s="4"/>
-      <c r="H124" s="5"/>
-      <c r="I124" s="5"/>
-      <c r="J124" s="4"/>
-      <c r="K124" s="4"/>
-      <c r="L124" s="4"/>
-      <c r="M124" s="4"/>
-      <c r="N124" s="5"/>
+      <c r="D124" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H124" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="I124" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="J124" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="K124" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L124" s="4">
+        <v>1690</v>
+      </c>
+      <c r="M124" s="4">
+        <v>30</v>
+      </c>
+      <c r="N124" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14">
+      <c r="A125" s="4">
+        <v>124</v>
+      </c>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="F125" s="6"/>
+      <c r="G125" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H125" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="I125" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J125" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="K125" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L125" s="4">
+        <v>1320</v>
+      </c>
+      <c r="M125" s="4">
+        <v>40</v>
+      </c>
+      <c r="N125" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14">
+      <c r="A126" s="4">
+        <v>125</v>
+      </c>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="F126" s="6"/>
+      <c r="G126" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H126" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="I126" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J126" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="K126" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L126" s="4">
+        <v>1250</v>
+      </c>
+      <c r="M126" s="4">
+        <v>60</v>
+      </c>
+      <c r="N126" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14">
+      <c r="A127" s="4">
+        <v>126</v>
+      </c>
+      <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
+      <c r="D127" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="F127" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="G127" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H127" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="I127" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J127" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="K127" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L127" s="4">
+        <v>1670</v>
+      </c>
+      <c r="M127" s="4">
+        <v>30</v>
+      </c>
+      <c r="N127" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14">
+      <c r="A128" s="4">
+        <v>127</v>
+      </c>
+      <c r="B128" s="4"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="F128" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="G128" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H128" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="I128" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J128" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="K128" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L128" s="4">
+        <v>1590</v>
+      </c>
+      <c r="M128" s="4">
+        <v>30</v>
+      </c>
+      <c r="N128" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14">
+      <c r="A129" s="4">
+        <v>128</v>
+      </c>
+      <c r="B129" s="4"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="G129" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H129" s="5" t="s">
+        <v>553</v>
+      </c>
+      <c r="I129" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J129" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="K129" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L129" s="4">
+        <v>1260</v>
+      </c>
+      <c r="M129" s="4">
+        <v>30</v>
+      </c>
+      <c r="N129" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14">
+      <c r="A130" s="4">
+        <v>129</v>
+      </c>
+      <c r="B130" s="4"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="G130" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H130" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="I130" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J130" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="K130" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L130" s="4">
+        <v>1560</v>
+      </c>
+      <c r="M130" s="4">
+        <v>40</v>
+      </c>
+      <c r="N130" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14">
+      <c r="A131" s="4">
+        <v>130</v>
+      </c>
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="F131" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="G131" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H131" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="I131" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J131" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="K131" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L131" s="4">
+        <v>1280</v>
+      </c>
+      <c r="M131" s="4">
+        <v>30</v>
+      </c>
+      <c r="N131" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14">
+      <c r="A132" s="4">
+        <v>131</v>
+      </c>
+      <c r="B132" s="4"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="G132" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H132" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="I132" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J132" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="K132" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L132" s="4">
+        <v>1520</v>
+      </c>
+      <c r="M132" s="4">
+        <v>30</v>
+      </c>
+      <c r="N132" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14">
+      <c r="A133" s="4">
+        <v>132</v>
+      </c>
+      <c r="B133" s="4"/>
+      <c r="C133" s="4"/>
+      <c r="D133" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="F133" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="G133" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H133" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="I133" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J133" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="K133" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L133" s="4">
+        <v>1360</v>
+      </c>
+      <c r="M133" s="4">
+        <v>50</v>
+      </c>
+      <c r="N133" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14">
+      <c r="A134" s="4">
+        <v>133</v>
+      </c>
+      <c r="B134" s="4"/>
+      <c r="C134" s="4"/>
+      <c r="D134" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="F134" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="G134" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H134" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="I134" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J134" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="K134" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L134" s="4">
+        <v>1300</v>
+      </c>
+      <c r="M134" s="4">
+        <v>30</v>
+      </c>
+      <c r="N134" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14">
+      <c r="A135" s="4">
+        <v>134</v>
+      </c>
+      <c r="B135" s="4"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="F135" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="G135" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H135" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="I135" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J135" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="K135" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L135" s="4">
+        <v>1570</v>
+      </c>
+      <c r="M135" s="4">
+        <v>30</v>
+      </c>
+      <c r="N135" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14">
+      <c r="A136" s="4">
+        <v>135</v>
+      </c>
+      <c r="B136" s="4"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="F136" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="G136" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="H136" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="I136" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J136" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="K136" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L136" s="4">
+        <v>1640</v>
+      </c>
+      <c r="M136" s="4">
+        <v>30</v>
+      </c>
+      <c r="N136" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14">
+      <c r="A137" s="4">
+        <v>136</v>
+      </c>
+      <c r="B137" s="4"/>
+      <c r="C137" s="4"/>
+      <c r="D137" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="F137" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="G137" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H137" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="I137" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J137" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="K137" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L137" s="4">
+        <v>1610</v>
+      </c>
+      <c r="M137" s="4">
+        <v>30</v>
+      </c>
+      <c r="N137" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14">
+      <c r="A138" s="4">
+        <v>137</v>
+      </c>
+      <c r="B138" s="4"/>
+      <c r="C138" s="4"/>
+      <c r="D138" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="F138" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="G138" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="H138" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="I138" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J138" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="K138" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L138" s="4">
+        <v>1550</v>
+      </c>
+      <c r="M138" s="4">
+        <v>30</v>
+      </c>
+      <c r="N138" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14">
+      <c r="A139" s="4">
+        <v>138</v>
+      </c>
+      <c r="B139" s="4"/>
+      <c r="C139" s="4"/>
+      <c r="D139" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="E139" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="F139" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="G139" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H139" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="I139" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J139" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="K139" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L139" s="4">
+        <v>1600</v>
+      </c>
+      <c r="M139" s="4">
+        <v>40</v>
+      </c>
+      <c r="N139" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14">
+      <c r="A140" s="4">
+        <v>139</v>
+      </c>
+      <c r="B140" s="4"/>
+      <c r="C140" s="4"/>
+      <c r="D140" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="F140" s="6"/>
+      <c r="G140" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H140" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="I140" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J140" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="K140" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L140" s="4">
+        <v>1590</v>
+      </c>
+      <c r="M140" s="4">
+        <v>30</v>
+      </c>
+      <c r="N140" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14">
+      <c r="A141" s="4">
+        <v>140</v>
+      </c>
+      <c r="B141" s="4"/>
+      <c r="C141" s="4"/>
+      <c r="D141" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="F141" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="G141" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H141" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="I141" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J141" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="K141" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L141" s="4">
+        <v>1300</v>
+      </c>
+      <c r="M141" s="4">
+        <v>40</v>
+      </c>
+      <c r="N141" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14">
+      <c r="A142" s="4">
+        <v>141</v>
+      </c>
+      <c r="B142" s="4"/>
+      <c r="C142" s="4"/>
+      <c r="D142" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="G142" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H142" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="I142" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J142" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="K142" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L142" s="4">
+        <v>1320</v>
+      </c>
+      <c r="M142" s="4">
+        <v>30</v>
+      </c>
+      <c r="N142" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14">
+      <c r="A143" s="4">
+        <v>142</v>
+      </c>
+      <c r="B143" s="4"/>
+      <c r="C143" s="4"/>
+      <c r="D143" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E143" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="F143" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="G143" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H143" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="I143" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J143" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="K143" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L143" s="4">
+        <v>1480</v>
+      </c>
+      <c r="M143" s="4">
+        <v>50</v>
+      </c>
+      <c r="N143" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14">
+      <c r="A144" s="4">
+        <v>143</v>
+      </c>
+      <c r="B144" s="4"/>
+      <c r="C144" s="4"/>
+      <c r="D144" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E144" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="F144" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="G144" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H144" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="I144" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J144" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="K144" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L144" s="4">
+        <v>1700</v>
+      </c>
+      <c r="M144" s="4">
+        <v>40</v>
+      </c>
+      <c r="N144" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14">
+      <c r="A145" s="4">
+        <v>144</v>
+      </c>
+      <c r="B145" s="4"/>
+      <c r="C145" s="4"/>
+      <c r="D145" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E145" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="F145" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="G145" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H145" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="I145" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J145" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="K145" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L145" s="4">
+        <v>1590</v>
+      </c>
+      <c r="M145" s="4">
+        <v>30</v>
+      </c>
+      <c r="N145" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14">
+      <c r="A146" s="4">
+        <v>145</v>
+      </c>
+      <c r="B146" s="4"/>
+      <c r="C146" s="4"/>
+      <c r="D146" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E146" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="F146" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="G146" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H146" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="I146" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J146" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="K146" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L146" s="4">
+        <v>1290</v>
+      </c>
+      <c r="M146" s="4">
+        <v>40</v>
+      </c>
+      <c r="N146" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14">
+      <c r="A147" s="4">
+        <v>146</v>
+      </c>
+      <c r="B147" s="4"/>
+      <c r="C147" s="4"/>
+      <c r="D147" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E147" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="F147" s="6"/>
+      <c r="G147" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="H147" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="I147" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J147" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="K147" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L147" s="4">
+        <v>1770</v>
+      </c>
+      <c r="M147" s="4">
+        <v>40</v>
+      </c>
+      <c r="N147" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14">
+      <c r="A148" s="4">
+        <v>147</v>
+      </c>
+      <c r="B148" s="4"/>
+      <c r="C148" s="4"/>
+      <c r="D148" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E148" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="F148" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="G148" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H148" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="I148" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J148" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="K148" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L148" s="4">
+        <v>1670</v>
+      </c>
+      <c r="M148" s="4">
+        <v>30</v>
+      </c>
+      <c r="N148" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14">
+      <c r="A149" s="4">
+        <v>148</v>
+      </c>
+      <c r="B149" s="4"/>
+      <c r="C149" s="4"/>
+      <c r="D149" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E149" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="F149" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="G149" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="H149" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="I149" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J149" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="K149" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L149" s="4">
+        <v>1640</v>
+      </c>
+      <c r="M149" s="4">
+        <v>30</v>
+      </c>
+      <c r="N149" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14">
+      <c r="A150" s="4">
+        <v>149</v>
+      </c>
+      <c r="B150" s="4"/>
+      <c r="C150" s="4"/>
+      <c r="D150" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E150" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="F150" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="G150" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="H150" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="I150" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J150" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="K150" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L150" s="4">
+        <v>1380</v>
+      </c>
+      <c r="M150" s="4">
+        <v>30</v>
+      </c>
+      <c r="N150" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14">
+      <c r="A151" s="4">
+        <v>150</v>
+      </c>
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+      <c r="D151" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E151" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="F151" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="G151" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H151" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="I151" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J151" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="K151" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L151" s="4">
+        <v>1770</v>
+      </c>
+      <c r="M151" s="4">
+        <v>40</v>
+      </c>
+      <c r="N151" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14">
+      <c r="A152" s="4">
+        <v>151</v>
+      </c>
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E152" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="F152" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="G152" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H152" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="I152" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J152" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="K152" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L152" s="4">
+        <v>1640</v>
+      </c>
+      <c r="M152" s="4">
+        <v>30</v>
+      </c>
+      <c r="N152" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14">
+      <c r="A153" s="4">
+        <v>152</v>
+      </c>
+      <c r="B153" s="4"/>
+      <c r="C153" s="4"/>
+      <c r="D153" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E153" s="20" t="s">
+        <v>467</v>
+      </c>
+      <c r="F153" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="G153" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H153" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="I153" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J153" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="K153" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L153" s="4">
+        <v>1610</v>
+      </c>
+      <c r="M153" s="4">
+        <v>30</v>
+      </c>
+      <c r="N153" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14">
+      <c r="A154" s="4">
+        <v>153</v>
+      </c>
+      <c r="B154" s="4"/>
+      <c r="C154" s="4"/>
+      <c r="D154" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E154" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="F154" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="G154" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H154" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="I154" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J154" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="K154" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L154" s="4">
+        <v>1590</v>
+      </c>
+      <c r="M154" s="4">
+        <v>30</v>
+      </c>
+      <c r="N154" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14">
+      <c r="A155" s="4">
+        <v>154</v>
+      </c>
+      <c r="B155" s="4"/>
+      <c r="C155" s="4"/>
+      <c r="D155" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E155" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="F155" s="6"/>
+      <c r="G155" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H155" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="I155" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J155" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="K155" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L155" s="4">
+        <v>1560</v>
+      </c>
+      <c r="M155" s="4">
+        <v>30</v>
+      </c>
+      <c r="N155" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14">
+      <c r="A156" s="4">
+        <v>155</v>
+      </c>
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+      <c r="D156" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E156" s="20" t="s">
+        <v>466</v>
+      </c>
+      <c r="F156" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="G156" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H156" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="I156" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J156" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="K156" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L156" s="4">
+        <v>1780</v>
+      </c>
+      <c r="M156" s="4">
+        <v>30</v>
+      </c>
+      <c r="N156" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14">
+      <c r="A157" s="4">
+        <v>156</v>
+      </c>
+      <c r="B157" s="4"/>
+      <c r="C157" s="4"/>
+      <c r="D157" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E157" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="F157" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="G157" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H157" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="I157" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J157" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="K157" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L157" s="4">
+        <v>1650</v>
+      </c>
+      <c r="M157" s="4">
+        <v>30</v>
+      </c>
+      <c r="N157" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14">
+      <c r="A158" s="4">
+        <v>157</v>
+      </c>
+      <c r="B158" s="4"/>
+      <c r="C158" s="4"/>
+      <c r="D158" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E158" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="F158" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="G158" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H158" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="I158" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J158" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="K158" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L158" s="4">
+        <v>1650</v>
+      </c>
+      <c r="M158" s="4">
+        <v>30</v>
+      </c>
+      <c r="N158" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14">
+      <c r="A159" s="4">
+        <v>158</v>
+      </c>
+      <c r="B159" s="4"/>
+      <c r="C159" s="4"/>
+      <c r="D159" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E159" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="F159" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="G159" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H159" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="I159" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J159" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="K159" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L159" s="4">
+        <v>1580</v>
+      </c>
+      <c r="M159" s="4">
+        <v>30</v>
+      </c>
+      <c r="N159" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14">
+      <c r="A160" s="4">
+        <v>159</v>
+      </c>
+      <c r="B160" s="4"/>
+      <c r="C160" s="4"/>
+      <c r="D160" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E160" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="F160" s="6"/>
+      <c r="G160" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H160" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="I160" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J160" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="K160" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L160" s="4">
+        <v>1560</v>
+      </c>
+      <c r="M160" s="4">
+        <v>30</v>
+      </c>
+      <c r="N160" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14">
+      <c r="A161" s="4">
+        <v>160</v>
+      </c>
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+      <c r="D161" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E161" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="F161" s="6"/>
+      <c r="G161" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H161" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="I161" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J161" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="K161" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L161" s="4">
+        <v>1520</v>
+      </c>
+      <c r="M161" s="4">
+        <v>30</v>
+      </c>
+      <c r="N161" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14">
+      <c r="A162" s="4">
+        <v>161</v>
+      </c>
+      <c r="B162" s="4"/>
+      <c r="C162" s="4"/>
+      <c r="D162" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E162" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F162" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="G162" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H162" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="I162" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J162" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="K162" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L162" s="4">
+        <v>1530</v>
+      </c>
+      <c r="M162" s="4">
+        <v>30</v>
+      </c>
+      <c r="N162" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14">
+      <c r="A163" s="4">
+        <v>162</v>
+      </c>
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
+      <c r="D163" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E163" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F163" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="G163" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H163" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="I163" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J163" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="K163" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L163" s="4">
+        <v>1570</v>
+      </c>
+      <c r="M163" s="4">
+        <v>30</v>
+      </c>
+      <c r="N163" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14">
+      <c r="A164" s="4">
+        <v>163</v>
+      </c>
+      <c r="B164" s="4"/>
+      <c r="C164" s="4"/>
+      <c r="D164" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E164" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F164" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="G164" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H164" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="I164" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J164" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="K164" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L164" s="4">
+        <v>1600</v>
+      </c>
+      <c r="M164" s="4">
+        <v>30</v>
+      </c>
+      <c r="N164" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14">
+      <c r="A165" s="4">
+        <v>164</v>
+      </c>
+      <c r="B165" s="4"/>
+      <c r="C165" s="4"/>
+      <c r="D165" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E165" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F165" s="6"/>
+      <c r="G165" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H165" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="I165" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J165" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="K165" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L165" s="4">
+        <v>1540</v>
+      </c>
+      <c r="M165" s="4">
+        <v>30</v>
+      </c>
+      <c r="N165" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14">
+      <c r="A166" s="4">
+        <v>165</v>
+      </c>
+      <c r="B166" s="4"/>
+      <c r="C166" s="4"/>
+      <c r="D166" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E166" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="F166" s="6"/>
+      <c r="G166" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H166" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I166" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J166" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="K166" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L166" s="4">
+        <v>1720</v>
+      </c>
+      <c r="M166" s="4">
+        <v>30</v>
+      </c>
+      <c r="N166" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14">
+      <c r="A167" s="4">
+        <v>166</v>
+      </c>
+      <c r="B167" s="4"/>
+      <c r="C167" s="4"/>
+      <c r="D167" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E167" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="F167" s="6"/>
+      <c r="G167" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H167" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="I167" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J167" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="K167" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L167" s="4">
+        <v>1650</v>
+      </c>
+      <c r="M167" s="4">
+        <v>30</v>
+      </c>
+      <c r="N167" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14">
+      <c r="A168" s="4">
+        <v>167</v>
+      </c>
+      <c r="B168" s="4"/>
+      <c r="C168" s="4"/>
+      <c r="D168" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E168" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="F168" s="6"/>
+      <c r="G168" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H168" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="I168" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J168" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="K168" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L168" s="4">
+        <v>1630</v>
+      </c>
+      <c r="M168" s="4">
+        <v>30</v>
+      </c>
+      <c r="N168" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14">
+      <c r="A169" s="4">
+        <v>168</v>
+      </c>
+      <c r="B169" s="4"/>
+      <c r="C169" s="4"/>
+      <c r="D169" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E169" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="F169" s="6"/>
+      <c r="G169" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H169" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="I169" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J169" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="K169" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L169" s="4">
+        <v>1630</v>
+      </c>
+      <c r="M169" s="4">
+        <v>40</v>
+      </c>
+      <c r="N169" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14">
+      <c r="A170" s="4">
+        <v>169</v>
+      </c>
+      <c r="B170" s="4"/>
+      <c r="C170" s="4"/>
+      <c r="D170" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E170" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="F170" s="6"/>
+      <c r="G170" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H170" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="I170" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J170" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="K170" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L170" s="4">
+        <v>1620</v>
+      </c>
+      <c r="M170" s="4">
+        <v>30</v>
+      </c>
+      <c r="N170" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14">
+      <c r="A171" s="4">
+        <v>170</v>
+      </c>
+      <c r="B171" s="4"/>
+      <c r="C171" s="4"/>
+      <c r="D171" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E171" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="F171" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="G171" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H171" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="I171" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J171" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="K171" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L171" s="4">
+        <v>1610</v>
+      </c>
+      <c r="M171" s="4">
+        <v>30</v>
+      </c>
+      <c r="N171" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14">
+      <c r="A172" s="4">
+        <v>171</v>
+      </c>
+      <c r="B172" s="4"/>
+      <c r="C172" s="4"/>
+      <c r="D172" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E172" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="F172" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="G172" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H172" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="I172" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J172" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="K172" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L172" s="4">
+        <v>1600</v>
+      </c>
+      <c r="M172" s="4">
+        <v>30</v>
+      </c>
+      <c r="N172" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14">
+      <c r="A173" s="4">
+        <v>172</v>
+      </c>
+      <c r="B173" s="4"/>
+      <c r="C173" s="4"/>
+      <c r="D173" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E173" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="F173" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="G173" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H173" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="I173" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J173" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="K173" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L173" s="4">
+        <v>1660</v>
+      </c>
+      <c r="M173" s="4">
+        <v>30</v>
+      </c>
+      <c r="N173" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14">
+      <c r="A174" s="4">
+        <v>173</v>
+      </c>
+      <c r="B174" s="4"/>
+      <c r="C174" s="4"/>
+      <c r="D174" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E174" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="F174" s="6"/>
+      <c r="G174" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H174" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="I174" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J174" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="K174" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L174" s="4">
+        <v>1640</v>
+      </c>
+      <c r="M174" s="4">
+        <v>30</v>
+      </c>
+      <c r="N174" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14">
+      <c r="A175" s="4">
+        <v>174</v>
+      </c>
+      <c r="B175" s="4"/>
+      <c r="C175" s="4"/>
+      <c r="D175" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E175" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="F175" s="6"/>
+      <c r="G175" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H175" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="I175" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J175" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="K175" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L175" s="4">
+        <v>1620</v>
+      </c>
+      <c r="M175" s="4">
+        <v>40</v>
+      </c>
+      <c r="N175" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14">
+      <c r="A176" s="4">
+        <v>175</v>
+      </c>
+      <c r="B176" s="4"/>
+      <c r="C176" s="4"/>
+      <c r="D176" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E176" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F176" s="6"/>
+      <c r="G176" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H176" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="I176" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J176" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="K176" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L176" s="4">
+        <v>1720</v>
+      </c>
+      <c r="M176" s="4">
+        <v>30</v>
+      </c>
+      <c r="N176" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14">
+      <c r="A177" s="4">
+        <v>176</v>
+      </c>
+      <c r="B177" s="4"/>
+      <c r="C177" s="4"/>
+      <c r="D177" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E177" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F177" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="G177" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H177" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="I177" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J177" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="K177" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L177" s="4">
+        <v>1530</v>
+      </c>
+      <c r="M177" s="4">
+        <v>30</v>
+      </c>
+      <c r="N177" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14">
+      <c r="A178" s="4">
+        <v>177</v>
+      </c>
+      <c r="B178" s="4"/>
+      <c r="C178" s="4"/>
+      <c r="D178" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E178" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="F178" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="G178" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H178" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="I178" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J178" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="K178" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L178" s="4">
+        <v>1710</v>
+      </c>
+      <c r="M178" s="4">
+        <v>30</v>
+      </c>
+      <c r="N178" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14">
+      <c r="A179" s="4">
+        <v>178</v>
+      </c>
+      <c r="B179" s="4"/>
+      <c r="C179" s="4"/>
+      <c r="D179" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E179" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="F179" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="G179" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H179" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="I179" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J179" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="K179" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L179" s="4">
+        <v>1670</v>
+      </c>
+      <c r="M179" s="4">
+        <v>30</v>
+      </c>
+      <c r="N179" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14">
+      <c r="A180" s="4">
+        <v>179</v>
+      </c>
+      <c r="B180" s="4"/>
+      <c r="C180" s="4"/>
+      <c r="D180" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E180" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="F180" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="G180" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H180" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="I180" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J180" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="K180" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L180" s="4">
+        <v>1760</v>
+      </c>
+      <c r="M180" s="4">
+        <v>30</v>
+      </c>
+      <c r="N180" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14">
+      <c r="A181" s="4">
+        <v>180</v>
+      </c>
+      <c r="B181" s="4"/>
+      <c r="C181" s="4"/>
+      <c r="D181" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E181" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="F181" s="6"/>
+      <c r="G181" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H181" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="I181" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J181" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="K181" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L181" s="4">
+        <v>1630</v>
+      </c>
+      <c r="M181" s="4">
+        <v>30</v>
+      </c>
+      <c r="N181" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14">
+      <c r="A182" s="4">
+        <v>181</v>
+      </c>
+      <c r="B182" s="4"/>
+      <c r="C182" s="4"/>
+      <c r="D182" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E182" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="F182" s="6"/>
+      <c r="G182" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H182" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="I182" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J182" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="K182" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L182" s="4">
+        <v>1620</v>
+      </c>
+      <c r="M182" s="4">
+        <v>40</v>
+      </c>
+      <c r="N182" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="183" spans="1:14">
+      <c r="A183" s="4">
+        <v>182</v>
+      </c>
+      <c r="B183" s="4"/>
+      <c r="C183" s="4"/>
+      <c r="D183" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E183" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="F183" s="6"/>
+      <c r="G183" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H183" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="I183" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J183" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="K183" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L183" s="4">
+        <v>1620</v>
+      </c>
+      <c r="M183" s="4">
+        <v>30</v>
+      </c>
+      <c r="N183" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="184" spans="1:14">
+      <c r="A184" s="4">
+        <v>183</v>
+      </c>
+      <c r="B184" s="4"/>
+      <c r="C184" s="4"/>
+      <c r="D184" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="E184" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="F184" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="G184" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="H184" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="I184" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J184" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="K184" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L184" s="4">
+        <v>1650</v>
+      </c>
+      <c r="M184" s="4">
+        <v>30</v>
+      </c>
+      <c r="N184" s="5" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14">
+      <c r="A185" s="4">
+        <v>184</v>
+      </c>
+      <c r="B185" s="4"/>
+      <c r="C185" s="4"/>
+      <c r="D185" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="E185" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="F185" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="G185" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="H185" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="I185" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J185" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="K185" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L185" s="4">
+        <v>1550</v>
+      </c>
+      <c r="M185" s="4">
+        <v>30</v>
+      </c>
+      <c r="N185" s="5" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="186" spans="1:14" ht="27">
+      <c r="A186" s="4">
+        <v>185</v>
+      </c>
+      <c r="B186" s="4"/>
+      <c r="C186" s="4"/>
+      <c r="D186" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="E186" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="F186" s="6" t="s">
+        <v>581</v>
+      </c>
+      <c r="G186" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="H186" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="I186" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J186" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="K186" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L186" s="4">
+        <v>1660</v>
+      </c>
+      <c r="M186" s="4">
+        <v>30</v>
+      </c>
+      <c r="N186" s="5" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14">
+      <c r="A187" s="4">
+        <v>186</v>
+      </c>
+      <c r="B187" s="4"/>
+      <c r="C187" s="4"/>
+      <c r="D187" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="E187" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="F187" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="G187" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="H187" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="I187" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J187" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="K187" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L187" s="4">
+        <v>1540</v>
+      </c>
+      <c r="M187" s="4">
+        <v>30</v>
+      </c>
+      <c r="N187" s="5" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="188" spans="1:14">
+      <c r="A188" s="4">
+        <v>187</v>
+      </c>
+      <c r="B188" s="4"/>
+      <c r="C188" s="4"/>
+      <c r="D188" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="E188" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="F188" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="G188" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="H188" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="I188" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J188" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="K188" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L188" s="4">
+        <v>1590</v>
+      </c>
+      <c r="M188" s="4">
+        <v>40</v>
+      </c>
+      <c r="N188" s="5" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14">
+      <c r="A189" s="4">
+        <v>188</v>
+      </c>
+      <c r="B189" s="4"/>
+      <c r="C189" s="4"/>
+      <c r="D189" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="E189" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="F189" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="G189" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="H189" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="I189" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J189" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="K189" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L189" s="4">
+        <v>1770</v>
+      </c>
+      <c r="M189" s="4">
+        <v>30</v>
+      </c>
+      <c r="N189" s="5" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14">
+      <c r="A190" s="4">
+        <v>189</v>
+      </c>
+      <c r="B190" s="4"/>
+      <c r="C190" s="4"/>
+      <c r="D190" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="E190" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="F190" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="G190" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="H190" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="I190" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J190" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="K190" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L190" s="4">
+        <v>1680</v>
+      </c>
+      <c r="M190" s="4">
+        <v>30</v>
+      </c>
+      <c r="N190" s="5" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14">
+      <c r="A191" s="4">
+        <v>190</v>
+      </c>
+      <c r="B191" s="4"/>
+      <c r="C191" s="4"/>
+      <c r="D191" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="E191" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="F191" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="G191" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="H191" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="I191" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J191" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="K191" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L191" s="4">
+        <v>1640</v>
+      </c>
+      <c r="M191" s="4">
+        <v>40</v>
+      </c>
+      <c r="N191" s="5" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14">
+      <c r="A192" s="4">
+        <v>191</v>
+      </c>
+      <c r="B192" s="4"/>
+      <c r="C192" s="4"/>
+      <c r="D192" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="E192" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="F192" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="G192" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="H192" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="I192" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J192" s="4"/>
+      <c r="K192" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L192" s="4">
+        <v>1630</v>
+      </c>
+      <c r="M192" s="4">
+        <v>30</v>
+      </c>
+      <c r="N192" s="5" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" ht="27">
+      <c r="A193" s="4">
+        <v>192</v>
+      </c>
+      <c r="B193" s="4"/>
+      <c r="C193" s="4"/>
+      <c r="D193" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="E193" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="F193" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="G193" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="H193" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="I193" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J193" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="K193" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L193" s="4">
+        <v>1660</v>
+      </c>
+      <c r="M193" s="4">
+        <v>30</v>
+      </c>
+      <c r="N193" s="5" t="s">
+        <v>610</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N124"/>
+  <autoFilter ref="A1:N124" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6727,11 +10415,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
@@ -6742,13 +10430,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>339</v>
       </c>
     </row>
@@ -6756,127 +10444,127 @@
       <c r="A2" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="15"/>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="16"/>
       <c r="B4" s="17" t="s">
+        <v>432</v>
+      </c>
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="C4" s="18"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="11" t="s">
-        <v>332</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="C7" s="12" t="s">
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>349</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>353</v>
+      <c r="C9" s="11" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="15"/>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>354</v>
+      <c r="C10" s="11" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="15"/>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>355</v>
+      <c r="C11" s="11" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="15"/>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>356</v>
+      <c r="C12" s="11" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="15"/>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>358</v>
+      <c r="C13" s="11" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="15"/>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>360</v>
+      <c r="C14" s="11" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
-        <v>359</v>
+        <v>433</v>
       </c>
       <c r="C15" s="18"/>
     </row>
@@ -6884,11 +10572,11 @@
       <c r="A16" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>357</v>
+      <c r="C16" s="11" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>